<commit_message>
modelo de Hilborn actualizado 9/9/2021
</commit_message>
<xml_diff>
--- a/surplus production model-SardAustralAysén.xlsx
+++ b/surplus production model-SardAustralAysén.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariajosezunigabasualto/MJZ/CTP2022/SARDINAAUSTRAL_AYSEN/PRIMER_INFORME/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5A1F26-6545-5840-918C-894EC5EAF978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B5B5B9-3EA2-8B4A-B51E-0ABA53B5F8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="260" yWindow="780" windowWidth="23180" windowHeight="21920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2579,7 +2579,7 @@
   <dimension ref="A1:T202"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -2777,7 +2777,7 @@
         <v>21973</v>
       </c>
       <c r="D11" s="18">
-        <f t="shared" ref="D11:D18" si="5">+D10+$B$3*D10*(1-(D10/$B$4))-B10</f>
+        <f t="shared" ref="D11:D17" si="5">+D10+$B$3*D10*(1-(D10/$B$4))-B10</f>
         <v>11537.347152106162</v>
       </c>
       <c r="E11" s="1">

</xml_diff>